<commit_message>
Changes pushed as part of Build#
</commit_message>
<xml_diff>
--- a/Utilities/data.xlsx
+++ b/Utilities/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\eclipse-workspace\SamplePOMProject\Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backups\Documents\SamplePOMProject\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -377,6 +377,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>